<commit_message>
gdp from csv update
not working yet; seems to be one extra unique product in both 30 and 43 that shows up as an extra row. Expecting 65 rows after dropping totals. Getting 66.
</commit_message>
<xml_diff>
--- a/scripts/OECD_Data_downloads/Table_43.xlsx
+++ b/scripts/OECD_Data_downloads/Table_43.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Horsting\Local_Only\Python_files\GTDR\Scripts\OECD_Data_downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Horsting\Local_Only\Python_files\GTDR\SUTs_data_quality_checks\scripts\OECD_Data_downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C501D4-3B4F-4328-AA48-9BC910A6584F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9A412F-5ED7-46CA-A0A6-179C2562D74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OECD.Stat export" sheetId="1" r:id="rId1"/>
@@ -1523,7 +1523,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1553,50 +1553,8 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="24" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -1606,6 +1564,15 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1643,17 +1610,62 @@
     <xf numFmtId="0" fontId="23" fillId="34" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="24" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2012,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CQ94"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BO2" workbookViewId="0">
-      <selection activeCell="CI13" sqref="CI13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BT2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2037,720 +2049,720 @@
       </c>
     </row>
     <row r="3" spans="1:95" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="41" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-      <c r="U3" s="42"/>
-      <c r="V3" s="42"/>
-      <c r="W3" s="42"/>
-      <c r="X3" s="42"/>
-      <c r="Y3" s="42"/>
-      <c r="Z3" s="42"/>
-      <c r="AA3" s="42"/>
-      <c r="AB3" s="42"/>
-      <c r="AC3" s="42"/>
-      <c r="AD3" s="42"/>
-      <c r="AE3" s="42"/>
-      <c r="AF3" s="42"/>
-      <c r="AG3" s="42"/>
-      <c r="AH3" s="42"/>
-      <c r="AI3" s="42"/>
-      <c r="AJ3" s="42"/>
-      <c r="AK3" s="42"/>
-      <c r="AL3" s="42"/>
-      <c r="AM3" s="42"/>
-      <c r="AN3" s="42"/>
-      <c r="AO3" s="42"/>
-      <c r="AP3" s="42"/>
-      <c r="AQ3" s="42"/>
-      <c r="AR3" s="42"/>
-      <c r="AS3" s="42"/>
-      <c r="AT3" s="42"/>
-      <c r="AU3" s="42"/>
-      <c r="AV3" s="42"/>
-      <c r="AW3" s="42"/>
-      <c r="AX3" s="42"/>
-      <c r="AY3" s="42"/>
-      <c r="AZ3" s="42"/>
-      <c r="BA3" s="42"/>
-      <c r="BB3" s="42"/>
-      <c r="BC3" s="42"/>
-      <c r="BD3" s="42"/>
-      <c r="BE3" s="42"/>
-      <c r="BF3" s="42"/>
-      <c r="BG3" s="42"/>
-      <c r="BH3" s="42"/>
-      <c r="BI3" s="42"/>
-      <c r="BJ3" s="42"/>
-      <c r="BK3" s="42"/>
-      <c r="BL3" s="42"/>
-      <c r="BM3" s="42"/>
-      <c r="BN3" s="42"/>
-      <c r="BO3" s="42"/>
-      <c r="BP3" s="42"/>
-      <c r="BQ3" s="42"/>
-      <c r="BR3" s="42"/>
-      <c r="BS3" s="42"/>
-      <c r="BT3" s="42"/>
-      <c r="BU3" s="42"/>
-      <c r="BV3" s="42"/>
-      <c r="BW3" s="42"/>
-      <c r="BX3" s="42"/>
-      <c r="BY3" s="42"/>
-      <c r="BZ3" s="42"/>
-      <c r="CA3" s="42"/>
-      <c r="CB3" s="42"/>
-      <c r="CC3" s="42"/>
-      <c r="CD3" s="42"/>
-      <c r="CE3" s="42"/>
-      <c r="CF3" s="42"/>
-      <c r="CG3" s="42"/>
-      <c r="CH3" s="42"/>
-      <c r="CI3" s="42"/>
-      <c r="CJ3" s="42"/>
-      <c r="CK3" s="42"/>
-      <c r="CL3" s="42"/>
-      <c r="CM3" s="42"/>
-      <c r="CN3" s="42"/>
-      <c r="CO3" s="42"/>
-      <c r="CP3" s="42"/>
-      <c r="CQ3" s="43"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="16"/>
+      <c r="Z3" s="16"/>
+      <c r="AA3" s="16"/>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="16"/>
+      <c r="AH3" s="16"/>
+      <c r="AI3" s="16"/>
+      <c r="AJ3" s="16"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="16"/>
+      <c r="AM3" s="16"/>
+      <c r="AN3" s="16"/>
+      <c r="AO3" s="16"/>
+      <c r="AP3" s="16"/>
+      <c r="AQ3" s="16"/>
+      <c r="AR3" s="16"/>
+      <c r="AS3" s="16"/>
+      <c r="AT3" s="16"/>
+      <c r="AU3" s="16"/>
+      <c r="AV3" s="16"/>
+      <c r="AW3" s="16"/>
+      <c r="AX3" s="16"/>
+      <c r="AY3" s="16"/>
+      <c r="AZ3" s="16"/>
+      <c r="BA3" s="16"/>
+      <c r="BB3" s="16"/>
+      <c r="BC3" s="16"/>
+      <c r="BD3" s="16"/>
+      <c r="BE3" s="16"/>
+      <c r="BF3" s="16"/>
+      <c r="BG3" s="16"/>
+      <c r="BH3" s="16"/>
+      <c r="BI3" s="16"/>
+      <c r="BJ3" s="16"/>
+      <c r="BK3" s="16"/>
+      <c r="BL3" s="16"/>
+      <c r="BM3" s="16"/>
+      <c r="BN3" s="16"/>
+      <c r="BO3" s="16"/>
+      <c r="BP3" s="16"/>
+      <c r="BQ3" s="16"/>
+      <c r="BR3" s="16"/>
+      <c r="BS3" s="16"/>
+      <c r="BT3" s="16"/>
+      <c r="BU3" s="16"/>
+      <c r="BV3" s="16"/>
+      <c r="BW3" s="16"/>
+      <c r="BX3" s="16"/>
+      <c r="BY3" s="16"/>
+      <c r="BZ3" s="16"/>
+      <c r="CA3" s="16"/>
+      <c r="CB3" s="16"/>
+      <c r="CC3" s="16"/>
+      <c r="CD3" s="16"/>
+      <c r="CE3" s="16"/>
+      <c r="CF3" s="16"/>
+      <c r="CG3" s="16"/>
+      <c r="CH3" s="16"/>
+      <c r="CI3" s="16"/>
+      <c r="CJ3" s="16"/>
+      <c r="CK3" s="16"/>
+      <c r="CL3" s="16"/>
+      <c r="CM3" s="16"/>
+      <c r="CN3" s="16"/>
+      <c r="CO3" s="16"/>
+      <c r="CP3" s="16"/>
+      <c r="CQ3" s="17"/>
     </row>
     <row r="4" spans="1:95" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
-      <c r="V4" s="30"/>
-      <c r="W4" s="30"/>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="30"/>
-      <c r="Z4" s="30"/>
-      <c r="AA4" s="30"/>
-      <c r="AB4" s="30"/>
-      <c r="AC4" s="30"/>
-      <c r="AD4" s="30"/>
-      <c r="AE4" s="30"/>
-      <c r="AF4" s="30"/>
-      <c r="AG4" s="30"/>
-      <c r="AH4" s="30"/>
-      <c r="AI4" s="30"/>
-      <c r="AJ4" s="30"/>
-      <c r="AK4" s="30"/>
-      <c r="AL4" s="30"/>
-      <c r="AM4" s="30"/>
-      <c r="AN4" s="30"/>
-      <c r="AO4" s="30"/>
-      <c r="AP4" s="30"/>
-      <c r="AQ4" s="30"/>
-      <c r="AR4" s="30"/>
-      <c r="AS4" s="30"/>
-      <c r="AT4" s="30"/>
-      <c r="AU4" s="30"/>
-      <c r="AV4" s="30"/>
-      <c r="AW4" s="30"/>
-      <c r="AX4" s="30"/>
-      <c r="AY4" s="30"/>
-      <c r="AZ4" s="30"/>
-      <c r="BA4" s="30"/>
-      <c r="BB4" s="30"/>
-      <c r="BC4" s="30"/>
-      <c r="BD4" s="30"/>
-      <c r="BE4" s="30"/>
-      <c r="BF4" s="30"/>
-      <c r="BG4" s="30"/>
-      <c r="BH4" s="30"/>
-      <c r="BI4" s="30"/>
-      <c r="BJ4" s="30"/>
-      <c r="BK4" s="30"/>
-      <c r="BL4" s="30"/>
-      <c r="BM4" s="30"/>
-      <c r="BN4" s="30"/>
-      <c r="BO4" s="30"/>
-      <c r="BP4" s="30"/>
-      <c r="BQ4" s="30"/>
-      <c r="BR4" s="30"/>
-      <c r="BS4" s="30"/>
-      <c r="BT4" s="30"/>
-      <c r="BU4" s="30"/>
-      <c r="BV4" s="30"/>
-      <c r="BW4" s="30"/>
-      <c r="BX4" s="30"/>
-      <c r="BY4" s="30"/>
-      <c r="BZ4" s="30"/>
-      <c r="CA4" s="30"/>
-      <c r="CB4" s="30"/>
-      <c r="CC4" s="30"/>
-      <c r="CD4" s="30"/>
-      <c r="CE4" s="30"/>
-      <c r="CF4" s="30"/>
-      <c r="CG4" s="30"/>
-      <c r="CH4" s="30"/>
-      <c r="CI4" s="30"/>
-      <c r="CJ4" s="30"/>
-      <c r="CK4" s="30"/>
-      <c r="CL4" s="30"/>
-      <c r="CM4" s="30"/>
-      <c r="CN4" s="30"/>
-      <c r="CO4" s="30"/>
-      <c r="CP4" s="30"/>
-      <c r="CQ4" s="31"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="19"/>
+      <c r="AE4" s="19"/>
+      <c r="AF4" s="19"/>
+      <c r="AG4" s="19"/>
+      <c r="AH4" s="19"/>
+      <c r="AI4" s="19"/>
+      <c r="AJ4" s="19"/>
+      <c r="AK4" s="19"/>
+      <c r="AL4" s="19"/>
+      <c r="AM4" s="19"/>
+      <c r="AN4" s="19"/>
+      <c r="AO4" s="19"/>
+      <c r="AP4" s="19"/>
+      <c r="AQ4" s="19"/>
+      <c r="AR4" s="19"/>
+      <c r="AS4" s="19"/>
+      <c r="AT4" s="19"/>
+      <c r="AU4" s="19"/>
+      <c r="AV4" s="19"/>
+      <c r="AW4" s="19"/>
+      <c r="AX4" s="19"/>
+      <c r="AY4" s="19"/>
+      <c r="AZ4" s="19"/>
+      <c r="BA4" s="19"/>
+      <c r="BB4" s="19"/>
+      <c r="BC4" s="19"/>
+      <c r="BD4" s="19"/>
+      <c r="BE4" s="19"/>
+      <c r="BF4" s="19"/>
+      <c r="BG4" s="19"/>
+      <c r="BH4" s="19"/>
+      <c r="BI4" s="19"/>
+      <c r="BJ4" s="19"/>
+      <c r="BK4" s="19"/>
+      <c r="BL4" s="19"/>
+      <c r="BM4" s="19"/>
+      <c r="BN4" s="19"/>
+      <c r="BO4" s="19"/>
+      <c r="BP4" s="19"/>
+      <c r="BQ4" s="19"/>
+      <c r="BR4" s="19"/>
+      <c r="BS4" s="19"/>
+      <c r="BT4" s="19"/>
+      <c r="BU4" s="19"/>
+      <c r="BV4" s="19"/>
+      <c r="BW4" s="19"/>
+      <c r="BX4" s="19"/>
+      <c r="BY4" s="19"/>
+      <c r="BZ4" s="19"/>
+      <c r="CA4" s="19"/>
+      <c r="CB4" s="19"/>
+      <c r="CC4" s="19"/>
+      <c r="CD4" s="19"/>
+      <c r="CE4" s="19"/>
+      <c r="CF4" s="19"/>
+      <c r="CG4" s="19"/>
+      <c r="CH4" s="19"/>
+      <c r="CI4" s="19"/>
+      <c r="CJ4" s="19"/>
+      <c r="CK4" s="19"/>
+      <c r="CL4" s="19"/>
+      <c r="CM4" s="19"/>
+      <c r="CN4" s="19"/>
+      <c r="CO4" s="19"/>
+      <c r="CP4" s="19"/>
+      <c r="CQ4" s="20"/>
     </row>
     <row r="5" spans="1:95" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="30"/>
-      <c r="T5" s="30"/>
-      <c r="U5" s="30"/>
-      <c r="V5" s="30"/>
-      <c r="W5" s="30"/>
-      <c r="X5" s="30"/>
-      <c r="Y5" s="30"/>
-      <c r="Z5" s="30"/>
-      <c r="AA5" s="30"/>
-      <c r="AB5" s="30"/>
-      <c r="AC5" s="30"/>
-      <c r="AD5" s="30"/>
-      <c r="AE5" s="30"/>
-      <c r="AF5" s="30"/>
-      <c r="AG5" s="30"/>
-      <c r="AH5" s="30"/>
-      <c r="AI5" s="30"/>
-      <c r="AJ5" s="30"/>
-      <c r="AK5" s="30"/>
-      <c r="AL5" s="30"/>
-      <c r="AM5" s="30"/>
-      <c r="AN5" s="30"/>
-      <c r="AO5" s="30"/>
-      <c r="AP5" s="30"/>
-      <c r="AQ5" s="30"/>
-      <c r="AR5" s="30"/>
-      <c r="AS5" s="30"/>
-      <c r="AT5" s="30"/>
-      <c r="AU5" s="30"/>
-      <c r="AV5" s="30"/>
-      <c r="AW5" s="30"/>
-      <c r="AX5" s="30"/>
-      <c r="AY5" s="30"/>
-      <c r="AZ5" s="30"/>
-      <c r="BA5" s="30"/>
-      <c r="BB5" s="30"/>
-      <c r="BC5" s="30"/>
-      <c r="BD5" s="30"/>
-      <c r="BE5" s="30"/>
-      <c r="BF5" s="30"/>
-      <c r="BG5" s="30"/>
-      <c r="BH5" s="30"/>
-      <c r="BI5" s="30"/>
-      <c r="BJ5" s="30"/>
-      <c r="BK5" s="30"/>
-      <c r="BL5" s="30"/>
-      <c r="BM5" s="30"/>
-      <c r="BN5" s="30"/>
-      <c r="BO5" s="30"/>
-      <c r="BP5" s="30"/>
-      <c r="BQ5" s="30"/>
-      <c r="BR5" s="30"/>
-      <c r="BS5" s="30"/>
-      <c r="BT5" s="30"/>
-      <c r="BU5" s="30"/>
-      <c r="BV5" s="30"/>
-      <c r="BW5" s="30"/>
-      <c r="BX5" s="30"/>
-      <c r="BY5" s="30"/>
-      <c r="BZ5" s="30"/>
-      <c r="CA5" s="30"/>
-      <c r="CB5" s="30"/>
-      <c r="CC5" s="30"/>
-      <c r="CD5" s="30"/>
-      <c r="CE5" s="30"/>
-      <c r="CF5" s="30"/>
-      <c r="CG5" s="30"/>
-      <c r="CH5" s="30"/>
-      <c r="CI5" s="30"/>
-      <c r="CJ5" s="30"/>
-      <c r="CK5" s="30"/>
-      <c r="CL5" s="30"/>
-      <c r="CM5" s="30"/>
-      <c r="CN5" s="30"/>
-      <c r="CO5" s="30"/>
-      <c r="CP5" s="30"/>
-      <c r="CQ5" s="31"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="19"/>
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="19"/>
+      <c r="AE5" s="19"/>
+      <c r="AF5" s="19"/>
+      <c r="AG5" s="19"/>
+      <c r="AH5" s="19"/>
+      <c r="AI5" s="19"/>
+      <c r="AJ5" s="19"/>
+      <c r="AK5" s="19"/>
+      <c r="AL5" s="19"/>
+      <c r="AM5" s="19"/>
+      <c r="AN5" s="19"/>
+      <c r="AO5" s="19"/>
+      <c r="AP5" s="19"/>
+      <c r="AQ5" s="19"/>
+      <c r="AR5" s="19"/>
+      <c r="AS5" s="19"/>
+      <c r="AT5" s="19"/>
+      <c r="AU5" s="19"/>
+      <c r="AV5" s="19"/>
+      <c r="AW5" s="19"/>
+      <c r="AX5" s="19"/>
+      <c r="AY5" s="19"/>
+      <c r="AZ5" s="19"/>
+      <c r="BA5" s="19"/>
+      <c r="BB5" s="19"/>
+      <c r="BC5" s="19"/>
+      <c r="BD5" s="19"/>
+      <c r="BE5" s="19"/>
+      <c r="BF5" s="19"/>
+      <c r="BG5" s="19"/>
+      <c r="BH5" s="19"/>
+      <c r="BI5" s="19"/>
+      <c r="BJ5" s="19"/>
+      <c r="BK5" s="19"/>
+      <c r="BL5" s="19"/>
+      <c r="BM5" s="19"/>
+      <c r="BN5" s="19"/>
+      <c r="BO5" s="19"/>
+      <c r="BP5" s="19"/>
+      <c r="BQ5" s="19"/>
+      <c r="BR5" s="19"/>
+      <c r="BS5" s="19"/>
+      <c r="BT5" s="19"/>
+      <c r="BU5" s="19"/>
+      <c r="BV5" s="19"/>
+      <c r="BW5" s="19"/>
+      <c r="BX5" s="19"/>
+      <c r="BY5" s="19"/>
+      <c r="BZ5" s="19"/>
+      <c r="CA5" s="19"/>
+      <c r="CB5" s="19"/>
+      <c r="CC5" s="19"/>
+      <c r="CD5" s="19"/>
+      <c r="CE5" s="19"/>
+      <c r="CF5" s="19"/>
+      <c r="CG5" s="19"/>
+      <c r="CH5" s="19"/>
+      <c r="CI5" s="19"/>
+      <c r="CJ5" s="19"/>
+      <c r="CK5" s="19"/>
+      <c r="CL5" s="19"/>
+      <c r="CM5" s="19"/>
+      <c r="CN5" s="19"/>
+      <c r="CO5" s="19"/>
+      <c r="CP5" s="19"/>
+      <c r="CQ5" s="20"/>
     </row>
     <row r="6" spans="1:95" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="30"/>
-      <c r="V6" s="30"/>
-      <c r="W6" s="30"/>
-      <c r="X6" s="30"/>
-      <c r="Y6" s="30"/>
-      <c r="Z6" s="30"/>
-      <c r="AA6" s="30"/>
-      <c r="AB6" s="30"/>
-      <c r="AC6" s="30"/>
-      <c r="AD6" s="30"/>
-      <c r="AE6" s="30"/>
-      <c r="AF6" s="30"/>
-      <c r="AG6" s="30"/>
-      <c r="AH6" s="30"/>
-      <c r="AI6" s="30"/>
-      <c r="AJ6" s="30"/>
-      <c r="AK6" s="30"/>
-      <c r="AL6" s="30"/>
-      <c r="AM6" s="30"/>
-      <c r="AN6" s="30"/>
-      <c r="AO6" s="30"/>
-      <c r="AP6" s="30"/>
-      <c r="AQ6" s="30"/>
-      <c r="AR6" s="30"/>
-      <c r="AS6" s="30"/>
-      <c r="AT6" s="30"/>
-      <c r="AU6" s="30"/>
-      <c r="AV6" s="30"/>
-      <c r="AW6" s="30"/>
-      <c r="AX6" s="30"/>
-      <c r="AY6" s="30"/>
-      <c r="AZ6" s="30"/>
-      <c r="BA6" s="30"/>
-      <c r="BB6" s="30"/>
-      <c r="BC6" s="30"/>
-      <c r="BD6" s="30"/>
-      <c r="BE6" s="30"/>
-      <c r="BF6" s="30"/>
-      <c r="BG6" s="30"/>
-      <c r="BH6" s="30"/>
-      <c r="BI6" s="30"/>
-      <c r="BJ6" s="30"/>
-      <c r="BK6" s="30"/>
-      <c r="BL6" s="30"/>
-      <c r="BM6" s="30"/>
-      <c r="BN6" s="30"/>
-      <c r="BO6" s="30"/>
-      <c r="BP6" s="30"/>
-      <c r="BQ6" s="30"/>
-      <c r="BR6" s="30"/>
-      <c r="BS6" s="30"/>
-      <c r="BT6" s="30"/>
-      <c r="BU6" s="30"/>
-      <c r="BV6" s="30"/>
-      <c r="BW6" s="30"/>
-      <c r="BX6" s="30"/>
-      <c r="BY6" s="30"/>
-      <c r="BZ6" s="30"/>
-      <c r="CA6" s="30"/>
-      <c r="CB6" s="30"/>
-      <c r="CC6" s="30"/>
-      <c r="CD6" s="30"/>
-      <c r="CE6" s="30"/>
-      <c r="CF6" s="30"/>
-      <c r="CG6" s="30"/>
-      <c r="CH6" s="30"/>
-      <c r="CI6" s="30"/>
-      <c r="CJ6" s="30"/>
-      <c r="CK6" s="30"/>
-      <c r="CL6" s="30"/>
-      <c r="CM6" s="30"/>
-      <c r="CN6" s="30"/>
-      <c r="CO6" s="30"/>
-      <c r="CP6" s="30"/>
-      <c r="CQ6" s="31"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="19"/>
+      <c r="AB6" s="19"/>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="19"/>
+      <c r="AE6" s="19"/>
+      <c r="AF6" s="19"/>
+      <c r="AG6" s="19"/>
+      <c r="AH6" s="19"/>
+      <c r="AI6" s="19"/>
+      <c r="AJ6" s="19"/>
+      <c r="AK6" s="19"/>
+      <c r="AL6" s="19"/>
+      <c r="AM6" s="19"/>
+      <c r="AN6" s="19"/>
+      <c r="AO6" s="19"/>
+      <c r="AP6" s="19"/>
+      <c r="AQ6" s="19"/>
+      <c r="AR6" s="19"/>
+      <c r="AS6" s="19"/>
+      <c r="AT6" s="19"/>
+      <c r="AU6" s="19"/>
+      <c r="AV6" s="19"/>
+      <c r="AW6" s="19"/>
+      <c r="AX6" s="19"/>
+      <c r="AY6" s="19"/>
+      <c r="AZ6" s="19"/>
+      <c r="BA6" s="19"/>
+      <c r="BB6" s="19"/>
+      <c r="BC6" s="19"/>
+      <c r="BD6" s="19"/>
+      <c r="BE6" s="19"/>
+      <c r="BF6" s="19"/>
+      <c r="BG6" s="19"/>
+      <c r="BH6" s="19"/>
+      <c r="BI6" s="19"/>
+      <c r="BJ6" s="19"/>
+      <c r="BK6" s="19"/>
+      <c r="BL6" s="19"/>
+      <c r="BM6" s="19"/>
+      <c r="BN6" s="19"/>
+      <c r="BO6" s="19"/>
+      <c r="BP6" s="19"/>
+      <c r="BQ6" s="19"/>
+      <c r="BR6" s="19"/>
+      <c r="BS6" s="19"/>
+      <c r="BT6" s="19"/>
+      <c r="BU6" s="19"/>
+      <c r="BV6" s="19"/>
+      <c r="BW6" s="19"/>
+      <c r="BX6" s="19"/>
+      <c r="BY6" s="19"/>
+      <c r="BZ6" s="19"/>
+      <c r="CA6" s="19"/>
+      <c r="CB6" s="19"/>
+      <c r="CC6" s="19"/>
+      <c r="CD6" s="19"/>
+      <c r="CE6" s="19"/>
+      <c r="CF6" s="19"/>
+      <c r="CG6" s="19"/>
+      <c r="CH6" s="19"/>
+      <c r="CI6" s="19"/>
+      <c r="CJ6" s="19"/>
+      <c r="CK6" s="19"/>
+      <c r="CL6" s="19"/>
+      <c r="CM6" s="19"/>
+      <c r="CN6" s="19"/>
+      <c r="CO6" s="19"/>
+      <c r="CP6" s="19"/>
+      <c r="CQ6" s="20"/>
     </row>
     <row r="7" spans="1:95" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="30"/>
-      <c r="V7" s="30"/>
-      <c r="W7" s="30"/>
-      <c r="X7" s="30"/>
-      <c r="Y7" s="30"/>
-      <c r="Z7" s="30"/>
-      <c r="AA7" s="30"/>
-      <c r="AB7" s="30"/>
-      <c r="AC7" s="30"/>
-      <c r="AD7" s="30"/>
-      <c r="AE7" s="30"/>
-      <c r="AF7" s="30"/>
-      <c r="AG7" s="30"/>
-      <c r="AH7" s="30"/>
-      <c r="AI7" s="30"/>
-      <c r="AJ7" s="30"/>
-      <c r="AK7" s="30"/>
-      <c r="AL7" s="30"/>
-      <c r="AM7" s="30"/>
-      <c r="AN7" s="30"/>
-      <c r="AO7" s="30"/>
-      <c r="AP7" s="30"/>
-      <c r="AQ7" s="30"/>
-      <c r="AR7" s="30"/>
-      <c r="AS7" s="30"/>
-      <c r="AT7" s="30"/>
-      <c r="AU7" s="30"/>
-      <c r="AV7" s="30"/>
-      <c r="AW7" s="30"/>
-      <c r="AX7" s="30"/>
-      <c r="AY7" s="30"/>
-      <c r="AZ7" s="30"/>
-      <c r="BA7" s="30"/>
-      <c r="BB7" s="30"/>
-      <c r="BC7" s="30"/>
-      <c r="BD7" s="30"/>
-      <c r="BE7" s="30"/>
-      <c r="BF7" s="30"/>
-      <c r="BG7" s="30"/>
-      <c r="BH7" s="30"/>
-      <c r="BI7" s="30"/>
-      <c r="BJ7" s="30"/>
-      <c r="BK7" s="30"/>
-      <c r="BL7" s="30"/>
-      <c r="BM7" s="30"/>
-      <c r="BN7" s="30"/>
-      <c r="BO7" s="30"/>
-      <c r="BP7" s="30"/>
-      <c r="BQ7" s="30"/>
-      <c r="BR7" s="30"/>
-      <c r="BS7" s="30"/>
-      <c r="BT7" s="30"/>
-      <c r="BU7" s="30"/>
-      <c r="BV7" s="30"/>
-      <c r="BW7" s="30"/>
-      <c r="BX7" s="30"/>
-      <c r="BY7" s="30"/>
-      <c r="BZ7" s="30"/>
-      <c r="CA7" s="30"/>
-      <c r="CB7" s="30"/>
-      <c r="CC7" s="30"/>
-      <c r="CD7" s="30"/>
-      <c r="CE7" s="30"/>
-      <c r="CF7" s="30"/>
-      <c r="CG7" s="30"/>
-      <c r="CH7" s="30"/>
-      <c r="CI7" s="30"/>
-      <c r="CJ7" s="30"/>
-      <c r="CK7" s="30"/>
-      <c r="CL7" s="30"/>
-      <c r="CM7" s="30"/>
-      <c r="CN7" s="30"/>
-      <c r="CO7" s="30"/>
-      <c r="CP7" s="30"/>
-      <c r="CQ7" s="31"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="19"/>
+      <c r="AB7" s="19"/>
+      <c r="AC7" s="19"/>
+      <c r="AD7" s="19"/>
+      <c r="AE7" s="19"/>
+      <c r="AF7" s="19"/>
+      <c r="AG7" s="19"/>
+      <c r="AH7" s="19"/>
+      <c r="AI7" s="19"/>
+      <c r="AJ7" s="19"/>
+      <c r="AK7" s="19"/>
+      <c r="AL7" s="19"/>
+      <c r="AM7" s="19"/>
+      <c r="AN7" s="19"/>
+      <c r="AO7" s="19"/>
+      <c r="AP7" s="19"/>
+      <c r="AQ7" s="19"/>
+      <c r="AR7" s="19"/>
+      <c r="AS7" s="19"/>
+      <c r="AT7" s="19"/>
+      <c r="AU7" s="19"/>
+      <c r="AV7" s="19"/>
+      <c r="AW7" s="19"/>
+      <c r="AX7" s="19"/>
+      <c r="AY7" s="19"/>
+      <c r="AZ7" s="19"/>
+      <c r="BA7" s="19"/>
+      <c r="BB7" s="19"/>
+      <c r="BC7" s="19"/>
+      <c r="BD7" s="19"/>
+      <c r="BE7" s="19"/>
+      <c r="BF7" s="19"/>
+      <c r="BG7" s="19"/>
+      <c r="BH7" s="19"/>
+      <c r="BI7" s="19"/>
+      <c r="BJ7" s="19"/>
+      <c r="BK7" s="19"/>
+      <c r="BL7" s="19"/>
+      <c r="BM7" s="19"/>
+      <c r="BN7" s="19"/>
+      <c r="BO7" s="19"/>
+      <c r="BP7" s="19"/>
+      <c r="BQ7" s="19"/>
+      <c r="BR7" s="19"/>
+      <c r="BS7" s="19"/>
+      <c r="BT7" s="19"/>
+      <c r="BU7" s="19"/>
+      <c r="BV7" s="19"/>
+      <c r="BW7" s="19"/>
+      <c r="BX7" s="19"/>
+      <c r="BY7" s="19"/>
+      <c r="BZ7" s="19"/>
+      <c r="CA7" s="19"/>
+      <c r="CB7" s="19"/>
+      <c r="CC7" s="19"/>
+      <c r="CD7" s="19"/>
+      <c r="CE7" s="19"/>
+      <c r="CF7" s="19"/>
+      <c r="CG7" s="19"/>
+      <c r="CH7" s="19"/>
+      <c r="CI7" s="19"/>
+      <c r="CJ7" s="19"/>
+      <c r="CK7" s="19"/>
+      <c r="CL7" s="19"/>
+      <c r="CM7" s="19"/>
+      <c r="CN7" s="19"/>
+      <c r="CO7" s="19"/>
+      <c r="CP7" s="19"/>
+      <c r="CQ7" s="20"/>
     </row>
     <row r="8" spans="1:95" x14ac:dyDescent="0.2">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="17" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="23"/>
-      <c r="X8" s="23"/>
-      <c r="Y8" s="23"/>
-      <c r="Z8" s="23"/>
-      <c r="AA8" s="23"/>
-      <c r="AB8" s="23"/>
-      <c r="AC8" s="23"/>
-      <c r="AD8" s="23"/>
-      <c r="AE8" s="23"/>
-      <c r="AF8" s="23"/>
-      <c r="AG8" s="23"/>
-      <c r="AH8" s="23"/>
-      <c r="AI8" s="23"/>
-      <c r="AJ8" s="23"/>
-      <c r="AK8" s="23"/>
-      <c r="AL8" s="23"/>
-      <c r="AM8" s="23"/>
-      <c r="AN8" s="23"/>
-      <c r="AO8" s="23"/>
-      <c r="AP8" s="23"/>
-      <c r="AQ8" s="23"/>
-      <c r="AR8" s="23"/>
-      <c r="AS8" s="23"/>
-      <c r="AT8" s="23"/>
-      <c r="AU8" s="23"/>
-      <c r="AV8" s="23"/>
-      <c r="AW8" s="23"/>
-      <c r="AX8" s="23"/>
-      <c r="AY8" s="23"/>
-      <c r="AZ8" s="23"/>
-      <c r="BA8" s="23"/>
-      <c r="BB8" s="23"/>
-      <c r="BC8" s="23"/>
-      <c r="BD8" s="23"/>
-      <c r="BE8" s="23"/>
-      <c r="BF8" s="23"/>
-      <c r="BG8" s="23"/>
-      <c r="BH8" s="23"/>
-      <c r="BI8" s="23"/>
-      <c r="BJ8" s="23"/>
-      <c r="BK8" s="23"/>
-      <c r="BL8" s="23"/>
-      <c r="BM8" s="23"/>
-      <c r="BN8" s="23"/>
-      <c r="BO8" s="23"/>
-      <c r="BP8" s="23"/>
-      <c r="BQ8" s="23"/>
-      <c r="BR8" s="23"/>
-      <c r="BS8" s="23"/>
-      <c r="BT8" s="23"/>
-      <c r="BU8" s="23"/>
-      <c r="BV8" s="23"/>
-      <c r="BW8" s="23"/>
-      <c r="BX8" s="23"/>
-      <c r="BY8" s="23"/>
-      <c r="BZ8" s="23"/>
-      <c r="CA8" s="23"/>
-      <c r="CB8" s="23"/>
-      <c r="CC8" s="23"/>
-      <c r="CD8" s="23"/>
-      <c r="CE8" s="23"/>
-      <c r="CF8" s="23"/>
-      <c r="CG8" s="23"/>
-      <c r="CH8" s="23"/>
-      <c r="CI8" s="23"/>
-      <c r="CJ8" s="23"/>
-      <c r="CK8" s="23"/>
-      <c r="CL8" s="23"/>
-      <c r="CM8" s="23"/>
-      <c r="CN8" s="23"/>
-      <c r="CO8" s="23"/>
-      <c r="CP8" s="23"/>
-      <c r="CQ8" s="24"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="34"/>
+      <c r="S8" s="34"/>
+      <c r="T8" s="34"/>
+      <c r="U8" s="34"/>
+      <c r="V8" s="34"/>
+      <c r="W8" s="34"/>
+      <c r="X8" s="34"/>
+      <c r="Y8" s="34"/>
+      <c r="Z8" s="34"/>
+      <c r="AA8" s="34"/>
+      <c r="AB8" s="34"/>
+      <c r="AC8" s="34"/>
+      <c r="AD8" s="34"/>
+      <c r="AE8" s="34"/>
+      <c r="AF8" s="34"/>
+      <c r="AG8" s="34"/>
+      <c r="AH8" s="34"/>
+      <c r="AI8" s="34"/>
+      <c r="AJ8" s="34"/>
+      <c r="AK8" s="34"/>
+      <c r="AL8" s="34"/>
+      <c r="AM8" s="34"/>
+      <c r="AN8" s="34"/>
+      <c r="AO8" s="34"/>
+      <c r="AP8" s="34"/>
+      <c r="AQ8" s="34"/>
+      <c r="AR8" s="34"/>
+      <c r="AS8" s="34"/>
+      <c r="AT8" s="34"/>
+      <c r="AU8" s="34"/>
+      <c r="AV8" s="34"/>
+      <c r="AW8" s="34"/>
+      <c r="AX8" s="34"/>
+      <c r="AY8" s="34"/>
+      <c r="AZ8" s="34"/>
+      <c r="BA8" s="34"/>
+      <c r="BB8" s="34"/>
+      <c r="BC8" s="34"/>
+      <c r="BD8" s="34"/>
+      <c r="BE8" s="34"/>
+      <c r="BF8" s="34"/>
+      <c r="BG8" s="34"/>
+      <c r="BH8" s="34"/>
+      <c r="BI8" s="34"/>
+      <c r="BJ8" s="34"/>
+      <c r="BK8" s="34"/>
+      <c r="BL8" s="34"/>
+      <c r="BM8" s="34"/>
+      <c r="BN8" s="34"/>
+      <c r="BO8" s="34"/>
+      <c r="BP8" s="34"/>
+      <c r="BQ8" s="34"/>
+      <c r="BR8" s="34"/>
+      <c r="BS8" s="34"/>
+      <c r="BT8" s="34"/>
+      <c r="BU8" s="34"/>
+      <c r="BV8" s="34"/>
+      <c r="BW8" s="34"/>
+      <c r="BX8" s="34"/>
+      <c r="BY8" s="34"/>
+      <c r="BZ8" s="34"/>
+      <c r="CA8" s="34"/>
+      <c r="CB8" s="34"/>
+      <c r="CC8" s="34"/>
+      <c r="CD8" s="34"/>
+      <c r="CE8" s="34"/>
+      <c r="CF8" s="34"/>
+      <c r="CG8" s="34"/>
+      <c r="CH8" s="34"/>
+      <c r="CI8" s="34"/>
+      <c r="CJ8" s="34"/>
+      <c r="CK8" s="34"/>
+      <c r="CL8" s="34"/>
+      <c r="CM8" s="34"/>
+      <c r="CN8" s="34"/>
+      <c r="CO8" s="34"/>
+      <c r="CP8" s="34"/>
+      <c r="CQ8" s="35"/>
     </row>
     <row r="9" spans="1:95" x14ac:dyDescent="0.2">
-      <c r="A9" s="35"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="17" t="s">
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="23"/>
-      <c r="Y9" s="23"/>
-      <c r="Z9" s="23"/>
-      <c r="AA9" s="23"/>
-      <c r="AB9" s="23"/>
-      <c r="AC9" s="23"/>
-      <c r="AD9" s="23"/>
-      <c r="AE9" s="23"/>
-      <c r="AF9" s="23"/>
-      <c r="AG9" s="23"/>
-      <c r="AH9" s="23"/>
-      <c r="AI9" s="23"/>
-      <c r="AJ9" s="23"/>
-      <c r="AK9" s="23"/>
-      <c r="AL9" s="23"/>
-      <c r="AM9" s="23"/>
-      <c r="AN9" s="23"/>
-      <c r="AO9" s="23"/>
-      <c r="AP9" s="23"/>
-      <c r="AQ9" s="23"/>
-      <c r="AR9" s="23"/>
-      <c r="AS9" s="23"/>
-      <c r="AT9" s="23"/>
-      <c r="AU9" s="23"/>
-      <c r="AV9" s="23"/>
-      <c r="AW9" s="23"/>
-      <c r="AX9" s="23"/>
-      <c r="AY9" s="23"/>
-      <c r="AZ9" s="23"/>
-      <c r="BA9" s="23"/>
-      <c r="BB9" s="23"/>
-      <c r="BC9" s="23"/>
-      <c r="BD9" s="23"/>
-      <c r="BE9" s="23"/>
-      <c r="BF9" s="23"/>
-      <c r="BG9" s="23"/>
-      <c r="BH9" s="23"/>
-      <c r="BI9" s="23"/>
-      <c r="BJ9" s="23"/>
-      <c r="BK9" s="23"/>
-      <c r="BL9" s="23"/>
-      <c r="BM9" s="23"/>
-      <c r="BN9" s="23"/>
-      <c r="BO9" s="23"/>
-      <c r="BP9" s="23"/>
-      <c r="BQ9" s="23"/>
-      <c r="BR9" s="23"/>
-      <c r="BS9" s="23"/>
-      <c r="BT9" s="23"/>
-      <c r="BU9" s="23"/>
-      <c r="BV9" s="23"/>
-      <c r="BW9" s="23"/>
-      <c r="BX9" s="23"/>
-      <c r="BY9" s="23"/>
-      <c r="BZ9" s="23"/>
-      <c r="CA9" s="23"/>
-      <c r="CB9" s="23"/>
-      <c r="CC9" s="23"/>
-      <c r="CD9" s="23"/>
-      <c r="CE9" s="23"/>
-      <c r="CF9" s="24"/>
-      <c r="CG9" s="17" t="s">
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="34"/>
+      <c r="T9" s="34"/>
+      <c r="U9" s="34"/>
+      <c r="V9" s="34"/>
+      <c r="W9" s="34"/>
+      <c r="X9" s="34"/>
+      <c r="Y9" s="34"/>
+      <c r="Z9" s="34"/>
+      <c r="AA9" s="34"/>
+      <c r="AB9" s="34"/>
+      <c r="AC9" s="34"/>
+      <c r="AD9" s="34"/>
+      <c r="AE9" s="34"/>
+      <c r="AF9" s="34"/>
+      <c r="AG9" s="34"/>
+      <c r="AH9" s="34"/>
+      <c r="AI9" s="34"/>
+      <c r="AJ9" s="34"/>
+      <c r="AK9" s="34"/>
+      <c r="AL9" s="34"/>
+      <c r="AM9" s="34"/>
+      <c r="AN9" s="34"/>
+      <c r="AO9" s="34"/>
+      <c r="AP9" s="34"/>
+      <c r="AQ9" s="34"/>
+      <c r="AR9" s="34"/>
+      <c r="AS9" s="34"/>
+      <c r="AT9" s="34"/>
+      <c r="AU9" s="34"/>
+      <c r="AV9" s="34"/>
+      <c r="AW9" s="34"/>
+      <c r="AX9" s="34"/>
+      <c r="AY9" s="34"/>
+      <c r="AZ9" s="34"/>
+      <c r="BA9" s="34"/>
+      <c r="BB9" s="34"/>
+      <c r="BC9" s="34"/>
+      <c r="BD9" s="34"/>
+      <c r="BE9" s="34"/>
+      <c r="BF9" s="34"/>
+      <c r="BG9" s="34"/>
+      <c r="BH9" s="34"/>
+      <c r="BI9" s="34"/>
+      <c r="BJ9" s="34"/>
+      <c r="BK9" s="34"/>
+      <c r="BL9" s="34"/>
+      <c r="BM9" s="34"/>
+      <c r="BN9" s="34"/>
+      <c r="BO9" s="34"/>
+      <c r="BP9" s="34"/>
+      <c r="BQ9" s="34"/>
+      <c r="BR9" s="34"/>
+      <c r="BS9" s="34"/>
+      <c r="BT9" s="34"/>
+      <c r="BU9" s="34"/>
+      <c r="BV9" s="34"/>
+      <c r="BW9" s="34"/>
+      <c r="BX9" s="34"/>
+      <c r="BY9" s="34"/>
+      <c r="BZ9" s="34"/>
+      <c r="CA9" s="34"/>
+      <c r="CB9" s="34"/>
+      <c r="CC9" s="34"/>
+      <c r="CD9" s="34"/>
+      <c r="CE9" s="34"/>
+      <c r="CF9" s="35"/>
+      <c r="CG9" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="CH9" s="22" t="s">
+      <c r="CH9" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="CI9" s="23"/>
-      <c r="CJ9" s="23"/>
-      <c r="CK9" s="24"/>
-      <c r="CL9" s="17" t="s">
+      <c r="CI9" s="34"/>
+      <c r="CJ9" s="34"/>
+      <c r="CK9" s="35"/>
+      <c r="CL9" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="CM9" s="22" t="s">
+      <c r="CM9" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="CN9" s="23"/>
-      <c r="CO9" s="24"/>
-      <c r="CP9" s="17" t="s">
+      <c r="CN9" s="34"/>
+      <c r="CO9" s="35"/>
+      <c r="CP9" s="30" t="s">
         <v>17</v>
       </c>
       <c r="CQ9" s="3" t="s">
@@ -2758,194 +2770,194 @@
       </c>
     </row>
     <row r="10" spans="1:95" ht="94.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="35"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="17" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="23"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="17" t="s">
+      <c r="I10" s="34"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="17" t="s">
+      <c r="L10" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="M10" s="22" t="s">
+      <c r="M10" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="23"/>
-      <c r="X10" s="23"/>
-      <c r="Y10" s="23"/>
-      <c r="Z10" s="23"/>
-      <c r="AA10" s="23"/>
-      <c r="AB10" s="23"/>
-      <c r="AC10" s="23"/>
-      <c r="AD10" s="23"/>
-      <c r="AE10" s="24"/>
-      <c r="AF10" s="17" t="s">
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="34"/>
+      <c r="T10" s="34"/>
+      <c r="U10" s="34"/>
+      <c r="V10" s="34"/>
+      <c r="W10" s="34"/>
+      <c r="X10" s="34"/>
+      <c r="Y10" s="34"/>
+      <c r="Z10" s="34"/>
+      <c r="AA10" s="34"/>
+      <c r="AB10" s="34"/>
+      <c r="AC10" s="34"/>
+      <c r="AD10" s="34"/>
+      <c r="AE10" s="35"/>
+      <c r="AF10" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="AG10" s="17" t="s">
+      <c r="AG10" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="AH10" s="22" t="s">
+      <c r="AH10" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="AI10" s="24"/>
-      <c r="AJ10" s="17" t="s">
+      <c r="AI10" s="35"/>
+      <c r="AJ10" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="AK10" s="17" t="s">
+      <c r="AK10" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="AL10" s="22" t="s">
+      <c r="AL10" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="AM10" s="23"/>
-      <c r="AN10" s="24"/>
-      <c r="AO10" s="17" t="s">
+      <c r="AM10" s="34"/>
+      <c r="AN10" s="35"/>
+      <c r="AO10" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="AP10" s="22" t="s">
+      <c r="AP10" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="AQ10" s="23"/>
-      <c r="AR10" s="23"/>
-      <c r="AS10" s="23"/>
-      <c r="AT10" s="24"/>
-      <c r="AU10" s="17" t="s">
+      <c r="AQ10" s="34"/>
+      <c r="AR10" s="34"/>
+      <c r="AS10" s="34"/>
+      <c r="AT10" s="35"/>
+      <c r="AU10" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="AV10" s="17" t="s">
+      <c r="AV10" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="AW10" s="22" t="s">
+      <c r="AW10" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="AX10" s="23"/>
-      <c r="AY10" s="23"/>
-      <c r="AZ10" s="24"/>
-      <c r="BA10" s="17" t="s">
+      <c r="AX10" s="34"/>
+      <c r="AY10" s="34"/>
+      <c r="AZ10" s="35"/>
+      <c r="BA10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="BB10" s="22" t="s">
+      <c r="BB10" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="BC10" s="23"/>
-      <c r="BD10" s="24"/>
-      <c r="BE10" s="17" t="s">
+      <c r="BC10" s="34"/>
+      <c r="BD10" s="35"/>
+      <c r="BE10" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="BF10" s="22" t="s">
+      <c r="BF10" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="BG10" s="24"/>
-      <c r="BH10" s="17" t="s">
+      <c r="BG10" s="35"/>
+      <c r="BH10" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="BI10" s="22" t="s">
+      <c r="BI10" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="BJ10" s="23"/>
-      <c r="BK10" s="23"/>
-      <c r="BL10" s="23"/>
-      <c r="BM10" s="24"/>
-      <c r="BN10" s="17" t="s">
+      <c r="BJ10" s="34"/>
+      <c r="BK10" s="34"/>
+      <c r="BL10" s="34"/>
+      <c r="BM10" s="35"/>
+      <c r="BN10" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="BO10" s="22" t="s">
+      <c r="BO10" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="BP10" s="23"/>
-      <c r="BQ10" s="23"/>
-      <c r="BR10" s="24"/>
-      <c r="BS10" s="17" t="s">
+      <c r="BP10" s="34"/>
+      <c r="BQ10" s="34"/>
+      <c r="BR10" s="35"/>
+      <c r="BS10" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="BT10" s="17" t="s">
+      <c r="BT10" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="BU10" s="17" t="s">
+      <c r="BU10" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="BV10" s="22" t="s">
+      <c r="BV10" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="BW10" s="24"/>
-      <c r="BX10" s="17" t="s">
+      <c r="BW10" s="35"/>
+      <c r="BX10" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="BY10" s="22" t="s">
+      <c r="BY10" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="BZ10" s="24"/>
-      <c r="CA10" s="17" t="s">
+      <c r="BZ10" s="35"/>
+      <c r="CA10" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="CB10" s="22" t="s">
+      <c r="CB10" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="CC10" s="23"/>
-      <c r="CD10" s="24"/>
-      <c r="CE10" s="17" t="s">
+      <c r="CC10" s="34"/>
+      <c r="CD10" s="35"/>
+      <c r="CE10" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="CF10" s="17" t="s">
+      <c r="CF10" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="CG10" s="25"/>
-      <c r="CH10" s="17" t="s">
+      <c r="CG10" s="46"/>
+      <c r="CH10" s="30" t="s">
         <v>39</v>
       </c>
       <c r="CI10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="CJ10" s="17" t="s">
+      <c r="CJ10" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="CK10" s="17" t="s">
+      <c r="CK10" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="CL10" s="25"/>
-      <c r="CM10" s="17" t="s">
+      <c r="CL10" s="46"/>
+      <c r="CM10" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="CN10" s="17" t="s">
+      <c r="CN10" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="CO10" s="17" t="s">
+      <c r="CO10" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="CP10" s="25"/>
-      <c r="CQ10" s="17" t="s">
+      <c r="CP10" s="31"/>
+      <c r="CQ10" s="45" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:95" ht="115.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="38"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+    <row r="11" spans="1:95" ht="120" x14ac:dyDescent="0.2">
+      <c r="A11" s="27"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="32"/>
       <c r="H11" s="3" t="s">
         <v>46</v>
       </c>
@@ -2955,8 +2967,8 @@
       <c r="J11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
       <c r="M11" s="3" t="s">
         <v>49</v>
       </c>
@@ -3014,16 +3026,16 @@
       <c r="AE11" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="AF11" s="18"/>
-      <c r="AG11" s="18"/>
+      <c r="AF11" s="32"/>
+      <c r="AG11" s="32"/>
       <c r="AH11" s="3" t="s">
         <v>68</v>
       </c>
       <c r="AI11" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="AJ11" s="18"/>
-      <c r="AK11" s="18"/>
+      <c r="AJ11" s="32"/>
+      <c r="AK11" s="32"/>
       <c r="AL11" s="3" t="s">
         <v>70</v>
       </c>
@@ -3033,7 +3045,7 @@
       <c r="AN11" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="AO11" s="18"/>
+      <c r="AO11" s="32"/>
       <c r="AP11" s="3" t="s">
         <v>73</v>
       </c>
@@ -3049,8 +3061,8 @@
       <c r="AT11" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AU11" s="18"/>
-      <c r="AV11" s="18"/>
+      <c r="AU11" s="32"/>
+      <c r="AV11" s="32"/>
       <c r="AW11" s="3" t="s">
         <v>78</v>
       </c>
@@ -3063,7 +3075,7 @@
       <c r="AZ11" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="BA11" s="18"/>
+      <c r="BA11" s="32"/>
       <c r="BB11" s="3" t="s">
         <v>82</v>
       </c>
@@ -3073,14 +3085,14 @@
       <c r="BD11" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="BE11" s="18"/>
+      <c r="BE11" s="32"/>
       <c r="BF11" s="3" t="s">
         <v>85</v>
       </c>
       <c r="BG11" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="BH11" s="18"/>
+      <c r="BH11" s="32"/>
       <c r="BI11" s="3" t="s">
         <v>87</v>
       </c>
@@ -3096,7 +3108,7 @@
       <c r="BM11" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="BN11" s="18"/>
+      <c r="BN11" s="32"/>
       <c r="BO11" s="3" t="s">
         <v>92</v>
       </c>
@@ -3109,23 +3121,23 @@
       <c r="BR11" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="BS11" s="18"/>
-      <c r="BT11" s="18"/>
-      <c r="BU11" s="18"/>
+      <c r="BS11" s="32"/>
+      <c r="BT11" s="32"/>
+      <c r="BU11" s="32"/>
       <c r="BV11" s="3" t="s">
         <v>96</v>
       </c>
       <c r="BW11" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="BX11" s="18"/>
+      <c r="BX11" s="32"/>
       <c r="BY11" s="3" t="s">
         <v>98</v>
       </c>
       <c r="BZ11" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="CA11" s="18"/>
+      <c r="CA11" s="32"/>
       <c r="CB11" s="3" t="s">
         <v>100</v>
       </c>
@@ -3135,28 +3147,28 @@
       <c r="CD11" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="CE11" s="18"/>
-      <c r="CF11" s="18"/>
-      <c r="CG11" s="18"/>
-      <c r="CH11" s="18"/>
-      <c r="CI11" s="3" t="s">
+      <c r="CE11" s="32"/>
+      <c r="CF11" s="32"/>
+      <c r="CG11" s="47"/>
+      <c r="CH11" s="32"/>
+      <c r="CI11" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="CJ11" s="18"/>
-      <c r="CK11" s="18"/>
-      <c r="CL11" s="18"/>
-      <c r="CM11" s="18"/>
-      <c r="CN11" s="18"/>
-      <c r="CO11" s="18"/>
-      <c r="CP11" s="18"/>
-      <c r="CQ11" s="18"/>
+      <c r="CJ11" s="32"/>
+      <c r="CK11" s="32"/>
+      <c r="CL11" s="47"/>
+      <c r="CM11" s="32"/>
+      <c r="CN11" s="32"/>
+      <c r="CO11" s="32"/>
+      <c r="CP11" s="32"/>
+      <c r="CQ11" s="47"/>
     </row>
     <row r="12" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="21"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="4" t="s">
         <v>105</v>
       </c>
@@ -3435,11 +3447,11 @@
       </c>
     </row>
     <row r="13" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="12"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="4" t="s">
         <v>106</v>
       </c>
@@ -3689,7 +3701,7 @@
       <c r="CH13" s="6">
         <v>348862</v>
       </c>
-      <c r="CI13" s="44">
+      <c r="CI13" s="11">
         <v>16593</v>
       </c>
       <c r="CJ13" s="6">
@@ -3718,13 +3730,13 @@
       </c>
     </row>
     <row r="14" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="40"/>
       <c r="D14" s="4" t="s">
         <v>106</v>
       </c>
@@ -4003,8 +4015,8 @@
       </c>
     </row>
     <row r="15" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="13" t="s">
+      <c r="A15" s="43"/>
+      <c r="B15" s="42" t="s">
         <v>108</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -4288,8 +4300,8 @@
       </c>
     </row>
     <row r="16" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="43"/>
       <c r="C16" s="5" t="s">
         <v>111</v>
       </c>
@@ -4571,8 +4583,8 @@
       </c>
     </row>
     <row r="17" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="14"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="44"/>
       <c r="C17" s="5" t="s">
         <v>112</v>
       </c>
@@ -4854,11 +4866,11 @@
       </c>
     </row>
     <row r="18" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="11" t="s">
+      <c r="A18" s="43"/>
+      <c r="B18" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="40"/>
       <c r="D18" s="4" t="s">
         <v>106</v>
       </c>
@@ -5137,11 +5149,11 @@
       </c>
     </row>
     <row r="19" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="11" t="s">
+      <c r="A19" s="43"/>
+      <c r="B19" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="40"/>
       <c r="D19" s="4" t="s">
         <v>106</v>
       </c>
@@ -5420,8 +5432,8 @@
       </c>
     </row>
     <row r="20" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="13" t="s">
+      <c r="A20" s="43"/>
+      <c r="B20" s="42" t="s">
         <v>114</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -5705,8 +5717,8 @@
       </c>
     </row>
     <row r="21" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
+      <c r="A21" s="43"/>
+      <c r="B21" s="43"/>
       <c r="C21" s="5" t="s">
         <v>116</v>
       </c>
@@ -5988,8 +6000,8 @@
       </c>
     </row>
     <row r="22" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
+      <c r="A22" s="43"/>
+      <c r="B22" s="43"/>
       <c r="C22" s="5" t="s">
         <v>117</v>
       </c>
@@ -6271,8 +6283,8 @@
       </c>
     </row>
     <row r="23" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="43"/>
       <c r="C23" s="5" t="s">
         <v>118</v>
       </c>
@@ -6554,8 +6566,8 @@
       </c>
     </row>
     <row r="24" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="43"/>
       <c r="C24" s="5" t="s">
         <v>119</v>
       </c>
@@ -6837,8 +6849,8 @@
       </c>
     </row>
     <row r="25" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="43"/>
       <c r="C25" s="5" t="s">
         <v>120</v>
       </c>
@@ -7120,8 +7132,8 @@
       </c>
     </row>
     <row r="26" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="43"/>
       <c r="C26" s="5" t="s">
         <v>121</v>
       </c>
@@ -7403,8 +7415,8 @@
       </c>
     </row>
     <row r="27" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="43"/>
+      <c r="B27" s="43"/>
       <c r="C27" s="5" t="s">
         <v>122</v>
       </c>
@@ -7686,8 +7698,8 @@
       </c>
     </row>
     <row r="28" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="43"/>
       <c r="C28" s="5" t="s">
         <v>123</v>
       </c>
@@ -7969,8 +7981,8 @@
       </c>
     </row>
     <row r="29" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="43"/>
+      <c r="B29" s="43"/>
       <c r="C29" s="5" t="s">
         <v>124</v>
       </c>
@@ -8252,8 +8264,8 @@
       </c>
     </row>
     <row r="30" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
+      <c r="A30" s="43"/>
+      <c r="B30" s="43"/>
       <c r="C30" s="5" t="s">
         <v>125</v>
       </c>
@@ -8535,8 +8547,8 @@
       </c>
     </row>
     <row r="31" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
+      <c r="A31" s="43"/>
+      <c r="B31" s="43"/>
       <c r="C31" s="5" t="s">
         <v>126</v>
       </c>
@@ -8818,8 +8830,8 @@
       </c>
     </row>
     <row r="32" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
+      <c r="A32" s="43"/>
+      <c r="B32" s="43"/>
       <c r="C32" s="5" t="s">
         <v>127</v>
       </c>
@@ -9101,8 +9113,8 @@
       </c>
     </row>
     <row r="33" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
+      <c r="A33" s="43"/>
+      <c r="B33" s="43"/>
       <c r="C33" s="5" t="s">
         <v>128</v>
       </c>
@@ -9384,8 +9396,8 @@
       </c>
     </row>
     <row r="34" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
+      <c r="A34" s="43"/>
+      <c r="B34" s="43"/>
       <c r="C34" s="5" t="s">
         <v>129</v>
       </c>
@@ -9667,8 +9679,8 @@
       </c>
     </row>
     <row r="35" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="43"/>
       <c r="C35" s="5" t="s">
         <v>130</v>
       </c>
@@ -9950,8 +9962,8 @@
       </c>
     </row>
     <row r="36" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="43"/>
       <c r="C36" s="5" t="s">
         <v>131</v>
       </c>
@@ -10233,8 +10245,8 @@
       </c>
     </row>
     <row r="37" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="43"/>
       <c r="C37" s="5" t="s">
         <v>132</v>
       </c>
@@ -10516,8 +10528,8 @@
       </c>
     </row>
     <row r="38" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="14"/>
+      <c r="A38" s="43"/>
+      <c r="B38" s="44"/>
       <c r="C38" s="5" t="s">
         <v>133</v>
       </c>
@@ -10799,11 +10811,11 @@
       </c>
     </row>
     <row r="39" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="11" t="s">
+      <c r="A39" s="43"/>
+      <c r="B39" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="C39" s="12"/>
+      <c r="C39" s="40"/>
       <c r="D39" s="4" t="s">
         <v>106</v>
       </c>
@@ -11082,11 +11094,11 @@
       </c>
     </row>
     <row r="40" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="11" t="s">
+      <c r="A40" s="43"/>
+      <c r="B40" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="C40" s="12"/>
+      <c r="C40" s="40"/>
       <c r="D40" s="4" t="s">
         <v>106</v>
       </c>
@@ -11365,8 +11377,8 @@
       </c>
     </row>
     <row r="41" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-      <c r="B41" s="13" t="s">
+      <c r="A41" s="43"/>
+      <c r="B41" s="42" t="s">
         <v>135</v>
       </c>
       <c r="C41" s="5" t="s">
@@ -11650,8 +11662,8 @@
       </c>
     </row>
     <row r="42" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="14"/>
+      <c r="A42" s="43"/>
+      <c r="B42" s="44"/>
       <c r="C42" s="5" t="s">
         <v>137</v>
       </c>
@@ -11933,11 +11945,11 @@
       </c>
     </row>
     <row r="43" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-      <c r="B43" s="11" t="s">
+      <c r="A43" s="43"/>
+      <c r="B43" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="C43" s="12"/>
+      <c r="C43" s="40"/>
       <c r="D43" s="4" t="s">
         <v>106</v>
       </c>
@@ -12216,11 +12228,11 @@
       </c>
     </row>
     <row r="44" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
-      <c r="B44" s="11" t="s">
+      <c r="A44" s="43"/>
+      <c r="B44" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="C44" s="12"/>
+      <c r="C44" s="40"/>
       <c r="D44" s="4" t="s">
         <v>106</v>
       </c>
@@ -12499,8 +12511,8 @@
       </c>
     </row>
     <row r="45" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="B45" s="13" t="s">
+      <c r="A45" s="43"/>
+      <c r="B45" s="42" t="s">
         <v>139</v>
       </c>
       <c r="C45" s="5" t="s">
@@ -12784,8 +12796,8 @@
       </c>
     </row>
     <row r="46" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
-      <c r="B46" s="15"/>
+      <c r="A46" s="43"/>
+      <c r="B46" s="43"/>
       <c r="C46" s="5" t="s">
         <v>141</v>
       </c>
@@ -13067,8 +13079,8 @@
       </c>
     </row>
     <row r="47" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
-      <c r="B47" s="14"/>
+      <c r="A47" s="43"/>
+      <c r="B47" s="44"/>
       <c r="C47" s="5" t="s">
         <v>142</v>
       </c>
@@ -13350,11 +13362,11 @@
       </c>
     </row>
     <row r="48" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
-      <c r="B48" s="11" t="s">
+      <c r="A48" s="43"/>
+      <c r="B48" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="C48" s="12"/>
+      <c r="C48" s="40"/>
       <c r="D48" s="4" t="s">
         <v>106</v>
       </c>
@@ -13633,8 +13645,8 @@
       </c>
     </row>
     <row r="49" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
-      <c r="B49" s="13" t="s">
+      <c r="A49" s="43"/>
+      <c r="B49" s="42" t="s">
         <v>143</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -13918,8 +13930,8 @@
       </c>
     </row>
     <row r="50" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
-      <c r="B50" s="15"/>
+      <c r="A50" s="43"/>
+      <c r="B50" s="43"/>
       <c r="C50" s="5" t="s">
         <v>145</v>
       </c>
@@ -14201,8 +14213,8 @@
       </c>
     </row>
     <row r="51" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
-      <c r="B51" s="15"/>
+      <c r="A51" s="43"/>
+      <c r="B51" s="43"/>
       <c r="C51" s="5" t="s">
         <v>146</v>
       </c>
@@ -14484,8 +14496,8 @@
       </c>
     </row>
     <row r="52" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
-      <c r="B52" s="15"/>
+      <c r="A52" s="43"/>
+      <c r="B52" s="43"/>
       <c r="C52" s="5" t="s">
         <v>147</v>
       </c>
@@ -14767,8 +14779,8 @@
       </c>
     </row>
     <row r="53" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
-      <c r="B53" s="14"/>
+      <c r="A53" s="43"/>
+      <c r="B53" s="44"/>
       <c r="C53" s="5" t="s">
         <v>148</v>
       </c>
@@ -15050,11 +15062,11 @@
       </c>
     </row>
     <row r="54" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
-      <c r="B54" s="11" t="s">
+      <c r="A54" s="43"/>
+      <c r="B54" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="C54" s="12"/>
+      <c r="C54" s="40"/>
       <c r="D54" s="4" t="s">
         <v>106</v>
       </c>
@@ -15333,11 +15345,11 @@
       </c>
     </row>
     <row r="55" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
-      <c r="B55" s="11" t="s">
+      <c r="A55" s="43"/>
+      <c r="B55" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="C55" s="12"/>
+      <c r="C55" s="40"/>
       <c r="D55" s="4" t="s">
         <v>106</v>
       </c>
@@ -15616,8 +15628,8 @@
       </c>
     </row>
     <row r="56" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
-      <c r="B56" s="13" t="s">
+      <c r="A56" s="43"/>
+      <c r="B56" s="42" t="s">
         <v>150</v>
       </c>
       <c r="C56" s="5" t="s">
@@ -15901,8 +15913,8 @@
       </c>
     </row>
     <row r="57" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A57" s="15"/>
-      <c r="B57" s="15"/>
+      <c r="A57" s="43"/>
+      <c r="B57" s="43"/>
       <c r="C57" s="5" t="s">
         <v>152</v>
       </c>
@@ -16184,8 +16196,8 @@
       </c>
     </row>
     <row r="58" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
-      <c r="B58" s="15"/>
+      <c r="A58" s="43"/>
+      <c r="B58" s="43"/>
       <c r="C58" s="5" t="s">
         <v>153</v>
       </c>
@@ -16467,8 +16479,8 @@
       </c>
     </row>
     <row r="59" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
-      <c r="B59" s="14"/>
+      <c r="A59" s="43"/>
+      <c r="B59" s="44"/>
       <c r="C59" s="5" t="s">
         <v>154</v>
       </c>
@@ -16750,11 +16762,11 @@
       </c>
     </row>
     <row r="60" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
-      <c r="B60" s="11" t="s">
+      <c r="A60" s="43"/>
+      <c r="B60" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="C60" s="12"/>
+      <c r="C60" s="40"/>
       <c r="D60" s="4" t="s">
         <v>106</v>
       </c>
@@ -17033,8 +17045,8 @@
       </c>
     </row>
     <row r="61" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
-      <c r="B61" s="13" t="s">
+      <c r="A61" s="43"/>
+      <c r="B61" s="42" t="s">
         <v>155</v>
       </c>
       <c r="C61" s="5" t="s">
@@ -17318,8 +17330,8 @@
       </c>
     </row>
     <row r="62" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
-      <c r="B62" s="15"/>
+      <c r="A62" s="43"/>
+      <c r="B62" s="43"/>
       <c r="C62" s="5" t="s">
         <v>157</v>
       </c>
@@ -17601,8 +17613,8 @@
       </c>
     </row>
     <row r="63" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="15"/>
-      <c r="B63" s="14"/>
+      <c r="A63" s="43"/>
+      <c r="B63" s="44"/>
       <c r="C63" s="5" t="s">
         <v>158</v>
       </c>
@@ -17884,11 +17896,11 @@
       </c>
     </row>
     <row r="64" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
-      <c r="B64" s="11" t="s">
+      <c r="A64" s="43"/>
+      <c r="B64" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="C64" s="12"/>
+      <c r="C64" s="40"/>
       <c r="D64" s="4" t="s">
         <v>106</v>
       </c>
@@ -18167,8 +18179,8 @@
       </c>
     </row>
     <row r="65" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A65" s="15"/>
-      <c r="B65" s="13" t="s">
+      <c r="A65" s="43"/>
+      <c r="B65" s="42" t="s">
         <v>159</v>
       </c>
       <c r="C65" s="5" t="s">
@@ -18452,8 +18464,8 @@
       </c>
     </row>
     <row r="66" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
-      <c r="B66" s="14"/>
+      <c r="A66" s="43"/>
+      <c r="B66" s="44"/>
       <c r="C66" s="5" t="s">
         <v>161</v>
       </c>
@@ -18735,11 +18747,11 @@
       </c>
     </row>
     <row r="67" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="15"/>
-      <c r="B67" s="11" t="s">
+      <c r="A67" s="43"/>
+      <c r="B67" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="C67" s="12"/>
+      <c r="C67" s="40"/>
       <c r="D67" s="4" t="s">
         <v>106</v>
       </c>
@@ -19018,8 +19030,8 @@
       </c>
     </row>
     <row r="68" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="15"/>
-      <c r="B68" s="13" t="s">
+      <c r="A68" s="43"/>
+      <c r="B68" s="42" t="s">
         <v>162</v>
       </c>
       <c r="C68" s="5" t="s">
@@ -19303,8 +19315,8 @@
       </c>
     </row>
     <row r="69" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="15"/>
-      <c r="B69" s="15"/>
+      <c r="A69" s="43"/>
+      <c r="B69" s="43"/>
       <c r="C69" s="5" t="s">
         <v>164</v>
       </c>
@@ -19586,8 +19598,8 @@
       </c>
     </row>
     <row r="70" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
-      <c r="B70" s="15"/>
+      <c r="A70" s="43"/>
+      <c r="B70" s="43"/>
       <c r="C70" s="5" t="s">
         <v>165</v>
       </c>
@@ -19869,8 +19881,8 @@
       </c>
     </row>
     <row r="71" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A71" s="15"/>
-      <c r="B71" s="15"/>
+      <c r="A71" s="43"/>
+      <c r="B71" s="43"/>
       <c r="C71" s="5" t="s">
         <v>166</v>
       </c>
@@ -20152,8 +20164,8 @@
       </c>
     </row>
     <row r="72" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="15"/>
-      <c r="B72" s="14"/>
+      <c r="A72" s="43"/>
+      <c r="B72" s="44"/>
       <c r="C72" s="5" t="s">
         <v>167</v>
       </c>
@@ -20435,11 +20447,11 @@
       </c>
     </row>
     <row r="73" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="15"/>
-      <c r="B73" s="11" t="s">
+      <c r="A73" s="43"/>
+      <c r="B73" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="C73" s="12"/>
+      <c r="C73" s="40"/>
       <c r="D73" s="4" t="s">
         <v>106</v>
       </c>
@@ -20718,8 +20730,8 @@
       </c>
     </row>
     <row r="74" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="15"/>
-      <c r="B74" s="13" t="s">
+      <c r="A74" s="43"/>
+      <c r="B74" s="42" t="s">
         <v>168</v>
       </c>
       <c r="C74" s="5" t="s">
@@ -21003,8 +21015,8 @@
       </c>
     </row>
     <row r="75" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="15"/>
-      <c r="B75" s="15"/>
+      <c r="A75" s="43"/>
+      <c r="B75" s="43"/>
       <c r="C75" s="5" t="s">
         <v>170</v>
       </c>
@@ -21286,8 +21298,8 @@
       </c>
     </row>
     <row r="76" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="15"/>
-      <c r="B76" s="15"/>
+      <c r="A76" s="43"/>
+      <c r="B76" s="43"/>
       <c r="C76" s="5" t="s">
         <v>171</v>
       </c>
@@ -21569,8 +21581,8 @@
       </c>
     </row>
     <row r="77" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
-      <c r="B77" s="14"/>
+      <c r="A77" s="43"/>
+      <c r="B77" s="44"/>
       <c r="C77" s="5" t="s">
         <v>172</v>
       </c>
@@ -21852,11 +21864,11 @@
       </c>
     </row>
     <row r="78" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="15"/>
-      <c r="B78" s="11" t="s">
+      <c r="A78" s="43"/>
+      <c r="B78" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="C78" s="12"/>
+      <c r="C78" s="40"/>
       <c r="D78" s="4" t="s">
         <v>106</v>
       </c>
@@ -22135,11 +22147,11 @@
       </c>
     </row>
     <row r="79" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="15"/>
-      <c r="B79" s="11" t="s">
+      <c r="A79" s="43"/>
+      <c r="B79" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="C79" s="12"/>
+      <c r="C79" s="40"/>
       <c r="D79" s="4" t="s">
         <v>106</v>
       </c>
@@ -22418,11 +22430,11 @@
       </c>
     </row>
     <row r="80" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="15"/>
-      <c r="B80" s="11" t="s">
+      <c r="A80" s="43"/>
+      <c r="B80" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="C80" s="12"/>
+      <c r="C80" s="40"/>
       <c r="D80" s="4" t="s">
         <v>106</v>
       </c>
@@ -22701,8 +22713,8 @@
       </c>
     </row>
     <row r="81" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="15"/>
-      <c r="B81" s="13" t="s">
+      <c r="A81" s="43"/>
+      <c r="B81" s="42" t="s">
         <v>175</v>
       </c>
       <c r="C81" s="5" t="s">
@@ -22986,8 +22998,8 @@
       </c>
     </row>
     <row r="82" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="15"/>
-      <c r="B82" s="14"/>
+      <c r="A82" s="43"/>
+      <c r="B82" s="44"/>
       <c r="C82" s="5" t="s">
         <v>177</v>
       </c>
@@ -23269,11 +23281,11 @@
       </c>
     </row>
     <row r="83" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A83" s="15"/>
-      <c r="B83" s="11" t="s">
+      <c r="A83" s="43"/>
+      <c r="B83" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="C83" s="12"/>
+      <c r="C83" s="40"/>
       <c r="D83" s="4" t="s">
         <v>106</v>
       </c>
@@ -23552,8 +23564,8 @@
       </c>
     </row>
     <row r="84" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="15"/>
-      <c r="B84" s="13" t="s">
+      <c r="A84" s="43"/>
+      <c r="B84" s="42" t="s">
         <v>178</v>
       </c>
       <c r="C84" s="5" t="s">
@@ -23837,8 +23849,8 @@
       </c>
     </row>
     <row r="85" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="15"/>
-      <c r="B85" s="14"/>
+      <c r="A85" s="43"/>
+      <c r="B85" s="44"/>
       <c r="C85" s="5" t="s">
         <v>180</v>
       </c>
@@ -24120,11 +24132,11 @@
       </c>
     </row>
     <row r="86" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="15"/>
-      <c r="B86" s="11" t="s">
+      <c r="A86" s="43"/>
+      <c r="B86" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="C86" s="12"/>
+      <c r="C86" s="40"/>
       <c r="D86" s="4" t="s">
         <v>106</v>
       </c>
@@ -24403,8 +24415,8 @@
       </c>
     </row>
     <row r="87" spans="1:95" ht="21" x14ac:dyDescent="0.25">
-      <c r="A87" s="15"/>
-      <c r="B87" s="13" t="s">
+      <c r="A87" s="43"/>
+      <c r="B87" s="42" t="s">
         <v>181</v>
       </c>
       <c r="C87" s="5" t="s">
@@ -24688,8 +24700,8 @@
       </c>
     </row>
     <row r="88" spans="1:95" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="15"/>
-      <c r="B88" s="15"/>
+      <c r="A88" s="43"/>
+      <c r="B88" s="43"/>
       <c r="C88" s="5" t="s">
         <v>183</v>
       </c>
@@ -24971,8 +24983,8 @@
       </c>
     </row>
     <row r="89" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A89" s="15"/>
-      <c r="B89" s="14"/>
+      <c r="A89" s="43"/>
+      <c r="B89" s="44"/>
       <c r="C89" s="5" t="s">
         <v>184</v>
       </c>
@@ -25254,11 +25266,11 @@
       </c>
     </row>
     <row r="90" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A90" s="15"/>
-      <c r="B90" s="11" t="s">
+      <c r="A90" s="43"/>
+      <c r="B90" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="C90" s="12"/>
+      <c r="C90" s="40"/>
       <c r="D90" s="4" t="s">
         <v>106</v>
       </c>
@@ -25537,11 +25549,11 @@
       </c>
     </row>
     <row r="91" spans="1:95" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="14"/>
-      <c r="B91" s="11" t="s">
+      <c r="A91" s="44"/>
+      <c r="B91" s="39" t="s">
         <v>186</v>
       </c>
-      <c r="C91" s="12"/>
+      <c r="C91" s="40"/>
       <c r="D91" s="4" t="s">
         <v>106</v>
       </c>
@@ -25839,12 +25851,82 @@
     </row>
   </sheetData>
   <mergeCells count="98">
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:CQ3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:CQ4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:CQ5"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:B85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B87:B89"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:B72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:A91"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:B38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:B53"/>
+    <mergeCell ref="CK10:CK11"/>
+    <mergeCell ref="CM10:CM11"/>
+    <mergeCell ref="CN10:CN11"/>
+    <mergeCell ref="CO10:CO11"/>
+    <mergeCell ref="CQ10:CQ11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="CA10:CA11"/>
+    <mergeCell ref="CB10:CD10"/>
+    <mergeCell ref="CE10:CE11"/>
+    <mergeCell ref="CF10:CF11"/>
+    <mergeCell ref="BE10:BE11"/>
+    <mergeCell ref="BF10:BG10"/>
+    <mergeCell ref="BH10:BH11"/>
+    <mergeCell ref="BI10:BM10"/>
+    <mergeCell ref="BN10:BN11"/>
+    <mergeCell ref="BO10:BR10"/>
+    <mergeCell ref="AP10:AT10"/>
+    <mergeCell ref="AU10:AU11"/>
+    <mergeCell ref="AV10:AV11"/>
+    <mergeCell ref="AW10:AZ10"/>
+    <mergeCell ref="BA10:BA11"/>
+    <mergeCell ref="CH10:CH11"/>
+    <mergeCell ref="CJ10:CJ11"/>
+    <mergeCell ref="BS10:BS11"/>
+    <mergeCell ref="BT10:BT11"/>
+    <mergeCell ref="BU10:BU11"/>
+    <mergeCell ref="BV10:BW10"/>
+    <mergeCell ref="BX10:BX11"/>
+    <mergeCell ref="BY10:BZ10"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:AE10"/>
+    <mergeCell ref="AF10:AF11"/>
+    <mergeCell ref="BB10:BD10"/>
+    <mergeCell ref="AG10:AG11"/>
+    <mergeCell ref="AH10:AI10"/>
+    <mergeCell ref="AJ10:AJ11"/>
+    <mergeCell ref="AK10:AK11"/>
+    <mergeCell ref="AL10:AN10"/>
+    <mergeCell ref="AO10:AO11"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="E6:CQ6"/>
     <mergeCell ref="A7:D7"/>
@@ -25861,82 +25943,12 @@
     <mergeCell ref="CP9:CP11"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:AE10"/>
-    <mergeCell ref="AF10:AF11"/>
-    <mergeCell ref="BB10:BD10"/>
-    <mergeCell ref="AG10:AG11"/>
-    <mergeCell ref="AH10:AI10"/>
-    <mergeCell ref="AJ10:AJ11"/>
-    <mergeCell ref="AK10:AK11"/>
-    <mergeCell ref="AL10:AN10"/>
-    <mergeCell ref="AO10:AO11"/>
-    <mergeCell ref="CH10:CH11"/>
-    <mergeCell ref="CJ10:CJ11"/>
-    <mergeCell ref="BS10:BS11"/>
-    <mergeCell ref="BT10:BT11"/>
-    <mergeCell ref="BU10:BU11"/>
-    <mergeCell ref="BV10:BW10"/>
-    <mergeCell ref="BX10:BX11"/>
-    <mergeCell ref="BY10:BZ10"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="CA10:CA11"/>
-    <mergeCell ref="CB10:CD10"/>
-    <mergeCell ref="CE10:CE11"/>
-    <mergeCell ref="CF10:CF11"/>
-    <mergeCell ref="BE10:BE11"/>
-    <mergeCell ref="BF10:BG10"/>
-    <mergeCell ref="BH10:BH11"/>
-    <mergeCell ref="BI10:BM10"/>
-    <mergeCell ref="BN10:BN11"/>
-    <mergeCell ref="BO10:BR10"/>
-    <mergeCell ref="AP10:AT10"/>
-    <mergeCell ref="AU10:AU11"/>
-    <mergeCell ref="AV10:AV11"/>
-    <mergeCell ref="AW10:AZ10"/>
-    <mergeCell ref="BA10:BA11"/>
-    <mergeCell ref="CK10:CK11"/>
-    <mergeCell ref="CM10:CM11"/>
-    <mergeCell ref="CN10:CN11"/>
-    <mergeCell ref="CO10:CO11"/>
-    <mergeCell ref="CQ10:CQ11"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:A91"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:B38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:B53"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:B72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:B77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:B85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B87:B89"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:CQ3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:CQ4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:CQ5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="http://localhost/OECDStat_Metadata/ShowMetadata.ashx?Dataset=SNA_TABLE40&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>